<commit_message>
Updated Pharma_stocks.xlsx with new data
</commit_message>
<xml_diff>
--- a/NAV/Pharma_stocks.xlsx
+++ b/NAV/Pharma_stocks.xlsx
@@ -450,7 +450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J596"/>
+  <dimension ref="A1:J617"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A583" workbookViewId="0">
       <selection activeCell="C597" sqref="C597"/>
@@ -18646,6 +18646,657 @@
     <row r="596">
       <c r="B596" s="5" t="n"/>
     </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>2024-08-28</t>
+        </is>
+      </c>
+      <c r="C597" t="n">
+        <v>2200.75</v>
+      </c>
+      <c r="D597" t="n">
+        <v>1539.5</v>
+      </c>
+      <c r="E597" t="n">
+        <v>1707.449951171875</v>
+      </c>
+      <c r="F597" t="n">
+        <v>1969.050048828125</v>
+      </c>
+      <c r="G597" t="n">
+        <v>1138.300048828125</v>
+      </c>
+      <c r="H597" t="n">
+        <v>8555.050048828125</v>
+      </c>
+      <c r="I597" t="n">
+        <v>0</v>
+      </c>
+      <c r="J597" t="n">
+        <v>195.3432372519036</v>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>2024-08-29</t>
+        </is>
+      </c>
+      <c r="C598" t="n">
+        <v>2193.75</v>
+      </c>
+      <c r="D598" t="n">
+        <v>1499.150024414062</v>
+      </c>
+      <c r="E598" t="n">
+        <v>1691.300048828125</v>
+      </c>
+      <c r="F598" t="n">
+        <v>1961.150024414062</v>
+      </c>
+      <c r="G598" t="n">
+        <v>1132.050048828125</v>
+      </c>
+      <c r="H598" t="n">
+        <v>8477.400146484375</v>
+      </c>
+      <c r="I598" t="n">
+        <v>-0.009076498898377167</v>
+      </c>
+      <c r="J598" t="n">
+        <v>193.5702045741812</v>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>2024-08-30</t>
+        </is>
+      </c>
+      <c r="C599" t="n">
+        <v>2240.199951171875</v>
+      </c>
+      <c r="D599" t="n">
+        <v>1537.550048828125</v>
+      </c>
+      <c r="E599" t="n">
+        <v>1731.75</v>
+      </c>
+      <c r="F599" t="n">
+        <v>1953.800048828125</v>
+      </c>
+      <c r="G599" t="n">
+        <v>1127.900024414062</v>
+      </c>
+      <c r="H599" t="n">
+        <v>8591.200073242188</v>
+      </c>
+      <c r="I599" t="n">
+        <v>0.01342391827581785</v>
+      </c>
+      <c r="J599" t="n">
+        <v>196.1686751810184</v>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>2024-09-02</t>
+        </is>
+      </c>
+      <c r="C600" t="n">
+        <v>2232.75</v>
+      </c>
+      <c r="D600" t="n">
+        <v>1537.550048828125</v>
+      </c>
+      <c r="E600" t="n">
+        <v>1687.900024414062</v>
+      </c>
+      <c r="F600" t="n">
+        <v>1970.599975585938</v>
+      </c>
+      <c r="G600" t="n">
+        <v>1111.550048828125</v>
+      </c>
+      <c r="H600" t="n">
+        <v>8540.35009765625</v>
+      </c>
+      <c r="I600" t="n">
+        <v>-0.005918844300264037</v>
+      </c>
+      <c r="J600" t="n">
+        <v>195.0075833360329</v>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>2024-09-03</t>
+        </is>
+      </c>
+      <c r="C601" t="n">
+        <v>2240.25</v>
+      </c>
+      <c r="D601" t="n">
+        <v>1530.599975585938</v>
+      </c>
+      <c r="E601" t="n">
+        <v>1687.5</v>
+      </c>
+      <c r="F601" t="n">
+        <v>1924.650024414062</v>
+      </c>
+      <c r="G601" t="n">
+        <v>1114</v>
+      </c>
+      <c r="H601" t="n">
+        <v>8497</v>
+      </c>
+      <c r="I601" t="n">
+        <v>-0.005075915759957742</v>
+      </c>
+      <c r="J601" t="n">
+        <v>194.0177412704662</v>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>2024-09-04</t>
+        </is>
+      </c>
+      <c r="C602" t="n">
+        <v>2277.25</v>
+      </c>
+      <c r="D602" t="n">
+        <v>1556.550048828125</v>
+      </c>
+      <c r="E602" t="n">
+        <v>1686.550048828125</v>
+      </c>
+      <c r="F602" t="n">
+        <v>1924.650024414062</v>
+      </c>
+      <c r="G602" t="n">
+        <v>1127.900024414062</v>
+      </c>
+      <c r="H602" t="n">
+        <v>8572.900146484375</v>
+      </c>
+      <c r="I602" t="n">
+        <v>0.008932581674046723</v>
+      </c>
+      <c r="J602" t="n">
+        <v>195.7508205905787</v>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>2024-09-05</t>
+        </is>
+      </c>
+      <c r="C603" t="n">
+        <v>2290.199951171875</v>
+      </c>
+      <c r="D603" t="n">
+        <v>1555.75</v>
+      </c>
+      <c r="E603" t="n">
+        <v>1709.449951171875</v>
+      </c>
+      <c r="F603" t="n">
+        <v>1933.599975585938</v>
+      </c>
+      <c r="G603" t="n">
+        <v>1115.150024414062</v>
+      </c>
+      <c r="H603" t="n">
+        <v>8604.14990234375</v>
+      </c>
+      <c r="I603" t="n">
+        <v>0.00364517903223101</v>
+      </c>
+      <c r="J603" t="n">
+        <v>196.4643673773375</v>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>2024-09-06</t>
+        </is>
+      </c>
+      <c r="C604" t="n">
+        <v>2256.5</v>
+      </c>
+      <c r="D604" t="n">
+        <v>1559.900024414062</v>
+      </c>
+      <c r="E604" t="n">
+        <v>1702.699951171875</v>
+      </c>
+      <c r="F604" t="n">
+        <v>1928.400024414062</v>
+      </c>
+      <c r="G604" t="n">
+        <v>1100</v>
+      </c>
+      <c r="H604" t="n">
+        <v>8547.5</v>
+      </c>
+      <c r="I604" t="n">
+        <v>-0.006584020848860234</v>
+      </c>
+      <c r="J604" t="n">
+        <v>195.170841886467</v>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>2024-09-09</t>
+        </is>
+      </c>
+      <c r="C605" t="n">
+        <v>2216.800048828125</v>
+      </c>
+      <c r="D605" t="n">
+        <v>1546.25</v>
+      </c>
+      <c r="E605" t="n">
+        <v>1704.199951171875</v>
+      </c>
+      <c r="F605" t="n">
+        <v>1937.099975585938</v>
+      </c>
+      <c r="G605" t="n">
+        <v>1104.150024414062</v>
+      </c>
+      <c r="H605" t="n">
+        <v>8508.5</v>
+      </c>
+      <c r="I605" t="n">
+        <v>-0.004562737642585551</v>
+      </c>
+      <c r="J605" t="n">
+        <v>194.2803285394565</v>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>2024-09-10</t>
+        </is>
+      </c>
+      <c r="C606" t="n">
+        <v>2222.550048828125</v>
+      </c>
+      <c r="D606" t="n">
+        <v>1545.550048828125</v>
+      </c>
+      <c r="E606" t="n">
+        <v>1727.849975585938</v>
+      </c>
+      <c r="F606" t="n">
+        <v>1912.150024414062</v>
+      </c>
+      <c r="G606" t="n">
+        <v>1113.199951171875</v>
+      </c>
+      <c r="H606" t="n">
+        <v>8521.300048828125</v>
+      </c>
+      <c r="I606" t="n">
+        <v>0.001504383713712758</v>
+      </c>
+      <c r="J606" t="n">
+        <v>194.572600701606</v>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>2024-09-11</t>
+        </is>
+      </c>
+      <c r="C607" t="n">
+        <v>2209.39990234375</v>
+      </c>
+      <c r="D607" t="n">
+        <v>1591.949951171875</v>
+      </c>
+      <c r="E607" t="n">
+        <v>1725.650024414062</v>
+      </c>
+      <c r="F607" t="n">
+        <v>1867.75</v>
+      </c>
+      <c r="G607" t="n">
+        <v>1112.599975585938</v>
+      </c>
+      <c r="H607" t="n">
+        <v>8507.349853515625</v>
+      </c>
+      <c r="I607" t="n">
+        <v>-0.001637097066476197</v>
+      </c>
+      <c r="J607" t="n">
+        <v>194.2540664677808</v>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>2024-09-12</t>
+        </is>
+      </c>
+      <c r="C608" t="n">
+        <v>2247.5</v>
+      </c>
+      <c r="D608" t="n">
+        <v>1592.849975585938</v>
+      </c>
+      <c r="E608" t="n">
+        <v>1747.949951171875</v>
+      </c>
+      <c r="F608" t="n">
+        <v>1883.349975585938</v>
+      </c>
+      <c r="G608" t="n">
+        <v>1120.099975585938</v>
+      </c>
+      <c r="H608" t="n">
+        <v>8591.749877929688</v>
+      </c>
+      <c r="I608" t="n">
+        <v>0.009920836202496664</v>
+      </c>
+      <c r="J608" t="n">
+        <v>196.1812292428765</v>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>2024-09-13</t>
+        </is>
+      </c>
+      <c r="C609" t="n">
+        <v>2256.449951171875</v>
+      </c>
+      <c r="D609" t="n">
+        <v>1582.5</v>
+      </c>
+      <c r="E609" t="n">
+        <v>1753.699951171875</v>
+      </c>
+      <c r="F609" t="n">
+        <v>1923.300048828125</v>
+      </c>
+      <c r="G609" t="n">
+        <v>1118.550048828125</v>
+      </c>
+      <c r="H609" t="n">
+        <v>8634.5</v>
+      </c>
+      <c r="I609" t="n">
+        <v>0.004975717714982386</v>
+      </c>
+      <c r="J609" t="n">
+        <v>197.1573716605673</v>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>2024-09-16</t>
+        </is>
+      </c>
+      <c r="C610" t="n">
+        <v>2251.85009765625</v>
+      </c>
+      <c r="D610" t="n">
+        <v>1577.75</v>
+      </c>
+      <c r="E610" t="n">
+        <v>1741.449951171875</v>
+      </c>
+      <c r="F610" t="n">
+        <v>1900.949951171875</v>
+      </c>
+      <c r="G610" t="n">
+        <v>1115.849975585938</v>
+      </c>
+      <c r="H610" t="n">
+        <v>8587.849975585938</v>
+      </c>
+      <c r="I610" t="n">
+        <v>-0.005402747630327465</v>
+      </c>
+      <c r="J610" t="n">
+        <v>196.0921801380266</v>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>2024-09-17</t>
+        </is>
+      </c>
+      <c r="C611" t="n">
+        <v>2270.39990234375</v>
+      </c>
+      <c r="D611" t="n">
+        <v>1561.699951171875</v>
+      </c>
+      <c r="E611" t="n">
+        <v>1713</v>
+      </c>
+      <c r="F611" t="n">
+        <v>1875.599975585938</v>
+      </c>
+      <c r="G611" t="n">
+        <v>1110.949951171875</v>
+      </c>
+      <c r="H611" t="n">
+        <v>8531.649780273438</v>
+      </c>
+      <c r="I611" t="n">
+        <v>-0.006544151967287428</v>
+      </c>
+      <c r="J611" t="n">
+        <v>194.8089231116067</v>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>2024-09-18</t>
+        </is>
+      </c>
+      <c r="C612" t="n">
+        <v>2224.949951171875</v>
+      </c>
+      <c r="D612" t="n">
+        <v>1543.050048828125</v>
+      </c>
+      <c r="E612" t="n">
+        <v>1646.050048828125</v>
+      </c>
+      <c r="F612" t="n">
+        <v>1857</v>
+      </c>
+      <c r="G612" t="n">
+        <v>1079.949951171875</v>
+      </c>
+      <c r="H612" t="n">
+        <v>8351</v>
+      </c>
+      <c r="I612" t="n">
+        <v>-0.02117407358786916</v>
+      </c>
+      <c r="J612" t="n">
+        <v>190.684024638068</v>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>2024-09-19</t>
+        </is>
+      </c>
+      <c r="C613" t="n">
+        <v>2171.89990234375</v>
+      </c>
+      <c r="D613" t="n">
+        <v>1515.050048828125</v>
+      </c>
+      <c r="E613" t="n">
+        <v>1649.800048828125</v>
+      </c>
+      <c r="F613" t="n">
+        <v>1886.5</v>
+      </c>
+      <c r="G613" t="n">
+        <v>1054.449951171875</v>
+      </c>
+      <c r="H613" t="n">
+        <v>8277.699951171875</v>
+      </c>
+      <c r="I613" t="n">
+        <v>-0.00877739777608969</v>
+      </c>
+      <c r="J613" t="n">
+        <v>189.010315104274</v>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>2024-09-20</t>
+        </is>
+      </c>
+      <c r="C614" t="n">
+        <v>2151.699951171875</v>
+      </c>
+      <c r="D614" t="n">
+        <v>1481.099975585938</v>
+      </c>
+      <c r="E614" t="n">
+        <v>1636.75</v>
+      </c>
+      <c r="F614" t="n">
+        <v>1897.25</v>
+      </c>
+      <c r="G614" t="n">
+        <v>1054.599975585938</v>
+      </c>
+      <c r="H614" t="n">
+        <v>8221.39990234375</v>
+      </c>
+      <c r="I614" t="n">
+        <v>-0.0068014121265841</v>
+      </c>
+      <c r="J614" t="n">
+        <v>187.7247780550743</v>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>2024-09-23</t>
+        </is>
+      </c>
+      <c r="C615" t="n">
+        <v>2182.25</v>
+      </c>
+      <c r="D615" t="n">
+        <v>1440.400024414062</v>
+      </c>
+      <c r="E615" t="n">
+        <v>1712.449951171875</v>
+      </c>
+      <c r="F615" t="n">
+        <v>1952</v>
+      </c>
+      <c r="G615" t="n">
+        <v>1055.25</v>
+      </c>
+      <c r="H615" t="n">
+        <v>8342.349975585938</v>
+      </c>
+      <c r="I615" t="n">
+        <v>0.01471161537923817</v>
+      </c>
+      <c r="J615" t="n">
+        <v>190.4865127869734</v>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>2024-09-24</t>
+        </is>
+      </c>
+      <c r="C616" t="n">
+        <v>2215.75</v>
+      </c>
+      <c r="D616" t="n">
+        <v>1414.25</v>
+      </c>
+      <c r="E616" t="n">
+        <v>1697.5</v>
+      </c>
+      <c r="F616" t="n">
+        <v>1944.349975585938</v>
+      </c>
+      <c r="G616" t="n">
+        <v>1051.550048828125</v>
+      </c>
+      <c r="H616" t="n">
+        <v>8323.400024414062</v>
+      </c>
+      <c r="I616" t="n">
+        <v>-0.002271536344954651</v>
+      </c>
+      <c r="J616" t="n">
+        <v>190.0538157499541</v>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>2024-09-25</t>
+        </is>
+      </c>
+      <c r="C617" t="n">
+        <v>2221.10009765625</v>
+      </c>
+      <c r="D617" t="n">
+        <v>1416.400024414062</v>
+      </c>
+      <c r="E617" t="n">
+        <v>1689.199951171875</v>
+      </c>
+      <c r="F617" t="n">
+        <v>1909.550048828125</v>
+      </c>
+      <c r="G617" t="n">
+        <v>1063.449951171875</v>
+      </c>
+      <c r="H617" t="n">
+        <v>8299.700073242188</v>
+      </c>
+      <c r="I617" t="n">
+        <v>-0.002847388219040138</v>
+      </c>
+      <c r="J617" t="n">
+        <v>189.512658754004</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>